<commit_message>
updated the bom to include the tread kit
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Github\WALL-E-Jr\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4A0E7F-7151-4B1A-A7DD-960EC4A27A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2D57ED-3D33-4AB0-B0FE-8AA25525E7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Part</t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.com/Aobao-Battery-Holder-Leads-Wires/dp/B09MZ1VFVY/ref=sr_1_15?keywords=AA+battery+case+with+wire+leads&amp;sr=8-15 </t>
+  </si>
+  <si>
+    <t>Tamiya Track and Wheel Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/Tamiya-Track-Wheel-Set-70100/dp/B001VZJDY2/ref=sr_1_1?keywords=Tamiya+Track+and+Wheel+Set&amp;sr=8-1 </t>
+  </si>
+  <si>
+    <t>Breadboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/Pcs-MCIGICM-Points-Solderless-Breadboard/dp/B07PCJP9DY/ref=sr_1_1_sspa?keywords=400+Tie-points+breadboard&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyTVRVVTE1NjBHVzVQJmVuY3J5cHRlZElkPUEwMjkzNDIxMTNHTTNMWDJENEw3NCZlbmNyeXB0ZWRBZElkPUEwMDM1MDQ2Mk4zR1VZSVU0NTJBMiZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU= </t>
+  </si>
+  <si>
+    <t>Basswood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/Hammont-Basswood-Sheets-12x8x1-Pack/dp/B09NWBMDNL/ref=sxin_17_ac_d_mf_brs?ac_md=3-1-SGFtbW9udA%3D%3D-ac_d_mf_brs_brs&amp;content-id=amzn1.sym.1ad31f34-ba12-4dca-be4b-f62f7f5bb10d%3Aamzn1.sym.1ad31f34-ba12-4dca-be4b-f62f7f5bb10d&amp;cv_ct_cx=basswood&amp;keywords=basswood&amp;pd_rd_i=B09NWBMDNL&amp;pd_rd_r=5220cbe5-6806-437d-863d-ca70e145ba67&amp;pd_rd_w=LW4Pl&amp;pd_rd_wg=ExU61&amp;pf_rd_p=1ad31f34-ba12-4dca-be4b-f62f7f5bb10d&amp;pf_rd_r=70TFQK3M4HVSSSABBFN7&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sr=1-2-8b2f235a-dddf-4202-bbb9-592393927392 </t>
   </si>
 </sst>
 </file>
@@ -148,18 +166,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -464,35 +475,35 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="2">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -500,10 +511,10 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="2">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -511,10 +522,10 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="2">
         <v>12</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -522,10 +533,10 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="2">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -533,10 +544,10 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -544,10 +555,10 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.5</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -555,10 +566,10 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -566,10 +577,10 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="2">
         <v>5</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -577,11 +588,44 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="2">
         <v>3</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -597,6 +641,9 @@
     <hyperlink ref="C10" r:id="rId9" display="https://www.amazon.com/WWZMDiB-TCRT5000-Reflective-Photoelectric-Avoidance/dp/B0BDDBM2TR/ref=sr_1_2_sspa?keywords=ir+sensor&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFRRlJCVFBFMkNUVTcmZW5jcnlwdGVkSWQ9QTA5NDE1MDYyUkEyNjNDVzJFOVpFJmVuY3J5cHRlZEFkSWQ9QTA5NTA0NjgyN1haUzZXOTlKMkI1JndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ== " xr:uid="{067DB3BF-09C2-48D7-9CBE-E0D8CE7F31A5}"/>
     <hyperlink ref="C11" r:id="rId10" display="https://www.amazon.com/Duracell-MN1500B4Z-CopperTop-Batteries-Technology/dp/B000YHO5MI/ref=sxin_18_ac_d_rm?ac_md=2-1-YWEgYmF0dGVyaWVzIGR1cmFjZWxs-ac_d_rm_rm_rm&amp;content-id=amzn1.sym.b09913c7-88ee-4b06-b977-3fd4ebd29a25%3Aamzn1.sym.b09913c7-88ee-4b06-b977-3fd4ebd29a25&amp;cv_ct_cx=AA+batteries&amp;keywords=AA+batteries&amp;pd_rd_i=B000YHO5MI&amp;pd_rd_r=04fa2ed3-a6a3-48fc-a495-c6c5a9c19a84&amp;pd_rd_w=YEVXp&amp;pd_rd_wg=yJezL&amp;pf_rd_p=b09913c7-88ee-4b06-b977-3fd4ebd29a25&amp;pf_rd_r=SHQMM0WSBVEYDAZKHTAV&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sr=1-2-7d9bfb42-6e38-4445-b604-42cab39e191b " xr:uid="{995230AD-642D-4F19-B1F6-424DACA13A73}"/>
     <hyperlink ref="C12" r:id="rId11" xr:uid="{CFA5CA48-5D1D-4284-891E-65A8342FE0DF}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{937F01A2-34E9-41B0-87A8-499EAAC2F9A4}"/>
+    <hyperlink ref="C14" r:id="rId13" display="https://www.amazon.com/Pcs-MCIGICM-Points-Solderless-Breadboard/dp/B07PCJP9DY/ref=sr_1_1_sspa?keywords=400+Tie-points+breadboard&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyTVRVVTE1NjBHVzVQJmVuY3J5cHRlZElkPUEwMjkzNDIxMTNHTTNMWDJENEw3NCZlbmNyeXB0ZWRBZElkPUEwMDM1MDQ2Mk4zR1VZSVU0NTJBMiZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU= " xr:uid="{B8AF80B1-F4A0-4814-8139-6EE91B4F6327}"/>
+    <hyperlink ref="C15" r:id="rId14" display="https://www.amazon.com/Hammont-Basswood-Sheets-12x8x1-Pack/dp/B09NWBMDNL/ref=sxin_17_ac_d_mf_brs?ac_md=3-1-SGFtbW9udA%3D%3D-ac_d_mf_brs_brs&amp;content-id=amzn1.sym.1ad31f34-ba12-4dca-be4b-f62f7f5bb10d%3Aamzn1.sym.1ad31f34-ba12-4dca-be4b-f62f7f5bb10d&amp;cv_ct_cx=basswood&amp;keywords=basswood&amp;pd_rd_i=B09NWBMDNL&amp;pd_rd_r=5220cbe5-6806-437d-863d-ca70e145ba67&amp;pd_rd_w=LW4Pl&amp;pd_rd_wg=ExU61&amp;pf_rd_p=1ad31f34-ba12-4dca-be4b-f62f7f5bb10d&amp;pf_rd_r=70TFQK3M4HVSSSABBFN7&amp;sbo=RZvfv%2F%2FHxDF%2BO5021pAnSA%3D%3D&amp;sr=1-2-8b2f235a-dddf-4202-bbb9-592393927392 " xr:uid="{608928CA-E729-4EB8-A98B-DA8E9EA20D57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>